<commit_message>
feat: importador Excel (SheetJS) + IndexedDB + recarga diaria (fix TS idb; ignore Excel lockfiles)
</commit_message>
<xml_diff>
--- a/public/dataset.xlsx
+++ b/public/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\english-trainer\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93210B04-F16A-4648-849C-269DBC636136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F740A553-910F-4D21-AF3B-81E58DBE1EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="280">
   <si>
     <t>Word/Expression</t>
   </si>
@@ -858,6 +858,12 @@
   </si>
   <si>
     <t>probable / adecuado</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -961,130 +967,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
+  <dxfs count="17">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFF9999"/>
           <bgColor rgb="FFFFB6C1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF9999"/>
-          <bgColor rgb="FFFFB6C1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99FF99"/>
-          <bgColor rgb="FFE6E6FA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99FF99"/>
-          <bgColor rgb="FFE6E6FA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-          <bgColor rgb="FFFFFACD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-          <bgColor rgb="FFFFFACD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCECFF"/>
-          <bgColor rgb="FFADD8E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCECFF"/>
-          <bgColor rgb="FFADD8E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-          <bgColor rgb="FFFFFACD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-          <bgColor rgb="FFFFFACD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCECFF"/>
-          <bgColor rgb="FFADD8E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCECFF"/>
-          <bgColor rgb="FFADD8E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFADD8E6"/>
-          <bgColor rgb="FFADD8E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FFE6E6FA"/>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1120,29 +1008,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFADD8E6"/>
-          <bgColor rgb="FFADD8E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFADD8E6"/>
-          <bgColor rgb="FFADD8E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <fgColor rgb="FFE6E6FA"/>
           <bgColor rgb="FF99FF99"/>
         </patternFill>
@@ -1166,128 +1031,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFADD8E6"/>
-          <bgColor rgb="FFADD8E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FFE6E6FA"/>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCECFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFADD8E6"/>
-          <bgColor rgb="FFADD8E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE6E6FA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB6C1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE6E6FA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB6C1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB6C1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE6E6FA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE6E6FA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFACD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFADD8E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB6C1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF98FB98"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1342,6 +1085,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFF9999"/>
+          <bgColor rgb="FFFFB6C1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFE6E6FA"/>
           <bgColor rgb="FFE6E6FA"/>
         </patternFill>
@@ -1375,18 +1126,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A2FA78BB-6E9B-4DC3-8066-61CDA510C17F}" name="Dict" displayName="Dict" ref="A1:F68" totalsRowShown="0" dataDxfId="45">
-  <autoFilter ref="A1:F68" xr:uid="{A2FA78BB-6E9B-4DC3-8066-61CDA510C17F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A2FA78BB-6E9B-4DC3-8066-61CDA510C17F}" name="Dict" displayName="Dict" ref="A1:F69" totalsRowShown="0" dataDxfId="16">
+  <autoFilter ref="A1:F69" xr:uid="{A2FA78BB-6E9B-4DC3-8066-61CDA510C17F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F68">
-    <sortCondition sortBy="cellColor" ref="D1:D68" dxfId="1"/>
+    <sortCondition sortBy="cellColor" ref="D1:D68" dxfId="15"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E8EDF67F-9004-4930-8BBF-AADD75CF9FFF}" name="Word/Expression" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{8E236CF7-DD74-44F6-B4B8-139F40D94CCC}" name="Definition (EN)" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{18FBB447-E87C-4D3E-A35E-E8AE8DA24001}" name="Example (EN)" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{38DC076B-96E3-4765-BA48-9D66D82126C9}" name="Translation (ES)" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{D24A6A44-07C8-4E68-97BE-CB55AF84196B}" name="Category" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{076348A4-7EC1-4E3E-A112-23D97A1F0EB6}" name="Seq" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{E8EDF67F-9004-4930-8BBF-AADD75CF9FFF}" name="Word/Expression" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{8E236CF7-DD74-44F6-B4B8-139F40D94CCC}" name="Definition (EN)" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{18FBB447-E87C-4D3E-A35E-E8AE8DA24001}" name="Example (EN)" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{38DC076B-96E3-4765-BA48-9D66D82126C9}" name="Translation (ES)" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{D24A6A44-07C8-4E68-97BE-CB55AF84196B}" name="Category" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{076348A4-7EC1-4E3E-A112-23D97A1F0EB6}" name="Seq" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1677,10 +1428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2920,37 +2671,53 @@
       </c>
       <c r="F68" s="7"/>
     </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F69" s="5"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:E67 A68:D68 A70:E10000">
-    <cfRule type="expression" dxfId="20" priority="1">
-      <formula>$E2="Verb"</formula>
+  <conditionalFormatting sqref="A69:D69">
+    <cfRule type="expression" dxfId="8" priority="6">
+      <formula>$D69="Verb"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="11">
+      <formula>$D69="Idiom"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="12">
+      <formula>$D69="Noun"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="13">
+      <formula>$D69="Adjective"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:E67 A68:D68 A70:E1000">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$E2="Idiom"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$E2="Noun"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$E2="Adjective"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A69:D69">
-    <cfRule type="expression" dxfId="16" priority="6">
-      <formula>$D69="Verb"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A69:D69">
-    <cfRule type="expression" dxfId="15" priority="11">
-      <formula>$D69="Idiom"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="12">
-      <formula>$D69="Noun"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="13">
-      <formula>$D69="Adjective"</formula>
+  <conditionalFormatting sqref="A2:E67 A68:D68 A70:E10000">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$E2="Verb"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>